<commit_message>
Gestión de reportes en asignación de cargos y estadística de tiempos laborados para las estructuras
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/appointments/Appointments.xlsx
+++ b/src/main/resources/reports/appointments/Appointments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS DOCUMENTOS\CIADTI\PROYECTOS\SERVICIOS\CARGA TRABAJO\ciadti-especifico-carga-trabajo-services\src\main\resources\reports\appointments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015FF5EB-5512-44AF-90D5-1638DA943FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F08F6C3-CB0C-4339-86A9-B4D099C5C994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle por dependencia" sheetId="2" r:id="rId1"/>
+    <sheet name="Comparativos" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,19 +50,19 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:area(lastCell="J12");
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="N9");
 jx:image(src="logo" lastCell="B3" imageType="PNG");</t>
         </r>
       </text>
@@ -74,19 +75,19 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:mergeCells(cols="size(levels) + treeDeep +6" rows="1" minCols="1" minRows="1" lastCell="C2");</t>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="totalCompensations+11" rows="1" minCols="1" minRows="1" lastCell="C2");</t>
         </r>
       </text>
     </comment>
@@ -98,19 +99,19 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:mergeCells(cols="size(levels) + treeDeep +6" rows="1" minCols="1" minRows="1" lastCell="C3");</t>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="totalCompensations+11" rows="1" minCols="1" minRows="1" lastCell="C3");</t>
         </r>
       </text>
     </comment>
@@ -134,79 +135,477 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:mergeCells(cols="treeDeep + size(levels) + 7" rows="1" minCols="1" minRows="1" lastCell="B5");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{A23335A4-ADDC-4440-AB6C-5E817460FCE6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:tree(tree="dataset" children="subEstructuras" nodeName="nombre" adjustBy="tipologia.nombre" nodeDescription="descripcion" areas=[B7:B8, C7:J8, B9:B9, C9:J9, B10:B11, C10:J11] lastCell="J11");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{6EF0F86E-7E59-4634-A2E8-FA2FE690FD55}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:merge(cols="size(levels)" rows="1" minCols="1" minRows="1" lastCell="J7");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{6ABF42C0-0F94-42A6-88E0-BE9CBFE1AB33}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="levels" var="level" lastCell="J8" direction="RIGHT");</t>
+jx:mergeCells(cols="totalCompensations + 12" rows="1" minCols="1" minRows="1" lastCell="B5");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{8722B099-0860-40A0-B269-49C91B659DA8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="categories" var="category" lastCell="M8" direction="RIGHT");
+jx:merge(cols="size(category.compensaciones)" rows="1" minCols="1" minRows="1" lastCell="M7");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{ADEBB074-C394-40AA-9F56-576C504E5E64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="category.compensaciones" var="compensation" lastCell="M8" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{2ACECE10-006B-4104-9D59-07E4ACA7544B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="dataset" var="scope" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{F5319C88-801F-4C8B-91D8-BE1A2647869F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="scope.children" var="validity" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{92997C66-2D07-4B7C-82E2-6BF7A0CE4182}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="validity.children" var="structure" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{0A3A7BAB-F781-4C63-9B7F-CBA921529458}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="structure.children" var="structureAppointment" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{BBA8CB56-BCD3-429D-B8F2-AFB6026544C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="structureAppointment.children" var="normativity" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{CF9ED112-5F62-4EBF-921E-19DDB76428CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="normativity.children" var="level" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{6414266E-9A2C-4C4C-9C05-2982714FE18C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="level.children" var="salaryScale" lastCell="N9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{305A5962-8E28-44AF-9F10-2329723ED3BA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="categories" var="category" lastCell="M9" direction="RIGHT");
+jx:each(items="category.compensaciones" var="compensation" lastCell="M9" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ronald Torres</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{505BF41D-03BA-48D8-98C7-913184D8989B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="E11");
+jx:image(src="logo" lastCell="B3" imageType="PNG");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{11B04264-326C-4469-B2B9-6AF1D31889D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols=" size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="C2");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{A8437416-A9C3-4A2B-97E6-3EE2FF0ED362}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols=" size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="C3");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{45650086-FC25-48B0-A8AF-2272253B9C45}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="1+size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="B5");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{CE9FAC1D-BF4D-4985-A473-EB1ECCA82FE5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="comparativesByScope" var="comparativeAttribute" lastCell="E8" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{1DD28C3D-ACC9-4964-9217-B9872A9CDD8E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="comparativeDataset" var="structure" lastCell="E11");
+jx:merge(cols="1 + size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="B9");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{1E3CEE09-E857-4793-B7B4-386B1C57C35C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="structure.children" var="level" lastCell="E10")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{CBA3538E-43DD-44C1-A687-0484FB8FE2BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="level.comparativesByScope" var="comparativeAttribute" lastCell="E10" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{558F7C05-BE3B-49DC-8394-F1B8703199AA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="comparativesByScope" var="comparativeAttribute" lastCell="E11" direction="RIGHT");</t>
         </r>
       </text>
     </comment>
@@ -215,52 +614,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>FRECUENCIA</t>
-  </si>
-  <si>
-    <t>Tmin</t>
-  </si>
-  <si>
-    <t>Tusual</t>
-  </si>
-  <si>
-    <t>Tmáx</t>
-  </si>
-  <si>
-    <t>TIEMPO TOTAL POR TAREA</t>
-  </si>
-  <si>
-    <t>TE (Tiempo Estandar)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Fecha del reporte:  ${reportDate}</t>
   </si>
   <si>
-    <t>$[UPPER(${"\"" + tittle + "\""})]</t>
-  </si>
-  <si>
-    <t>$[UPPER(${"\"" + level.nomenclatura + "\""})]</t>
-  </si>
-  <si>
-    <t>Designación de cargos</t>
-  </si>
-  <si>
-    <t>Cargos designados por dependencia en cada vigencia</t>
-  </si>
-  <si>
     <t>N° DE CARGOS</t>
   </si>
   <si>
-    <t>ASIGNACIÓN BÁSICA</t>
+    <t>Cargos asignados por dependencia en cada vigencia</t>
+  </si>
+  <si>
+    <t>ALCANCE</t>
+  </si>
+  <si>
+    <t>DEPENDENCIA</t>
+  </si>
+  <si>
+    <t>ACUERDO</t>
+  </si>
+  <si>
+    <t>NIVEL OCUPACIONAL</t>
+  </si>
+  <si>
+    <t>ESCALA SALARIAL</t>
+  </si>
+  <si>
+    <t>CÓDIGO</t>
+  </si>
+  <si>
+    <t>ASIGNACIÓN</t>
+  </si>
+  <si>
+    <t>VIGENCIA</t>
+  </si>
+  <si>
+    <t>${validity.data.nombre}</t>
+  </si>
+  <si>
+    <t>${structure.data.nombre}</t>
+  </si>
+  <si>
+    <t>${normativity.data.nombre}</t>
+  </si>
+  <si>
+    <t>${level.data.descripcion}</t>
+  </si>
+  <si>
+    <t>${salaryScale.data.nombre}</t>
+  </si>
+  <si>
+    <t>${salaryScale.data.codigo}</t>
+  </si>
+  <si>
+    <t>TOTAL DE CARGOS</t>
+  </si>
+  <si>
+    <t>$[K9*12]</t>
+  </si>
+  <si>
+    <t>$[UPPER(${"\"" +scope.data.nombre + "\""})]</t>
+  </si>
+  <si>
+    <t>${compensation.nombre}</t>
+  </si>
+  <si>
+    <t>${structureAppointment.totalCargos}</t>
+  </si>
+  <si>
+    <t>${salaryScale.totalCargos}</t>
+  </si>
+  <si>
+    <t>${salaryScale.asignacionBasicaMensual}</t>
+  </si>
+  <si>
+    <t>${salaryScale.valueByCompensation[compensation.id]}</t>
+  </si>
+  <si>
+    <t>Asignación básica mensual</t>
+  </si>
+  <si>
+    <t>Asignación básica anual</t>
+  </si>
+  <si>
+    <t>$[UPPER(${"\"" +category.nombre + "\""})]</t>
+  </si>
+  <si>
+    <t>TOTAL ANUAL</t>
+  </si>
+  <si>
+    <t>$[SUM(M9, L9)*J9]</t>
+  </si>
+  <si>
+    <t>$[UPPER(${"\"" +structure.data.nombre + "\""})]</t>
+  </si>
+  <si>
+    <t>${level.data.nombre}</t>
+  </si>
+  <si>
+    <t>Total de cargos</t>
+  </si>
+  <si>
+    <t>$[UPPER(${"\"" +comparativeAttribute.name + "\""})]</t>
+  </si>
+  <si>
+    <t>${comparativeAttribute.totalCargos}</t>
+  </si>
+  <si>
+    <t>${comparativeAttribute.asignacionBasicaAnual}</t>
+  </si>
+  <si>
+    <t>$[D10/12]</t>
+  </si>
+  <si>
+    <t>Comparativo de costos por alcances operativos en las dependencias por niveles ocupacionales</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>${R.sumComparativesByScope(structure.children, comparativeAttribute.key, 'asignacionBasicaAnual')}</t>
+  </si>
+  <si>
+    <t>${R.sumComparativesByScope(structure.children, comparativeAttribute.key, 'totalCargos')}</t>
+  </si>
+  <si>
+    <t>$[D11/12]</t>
+  </si>
+  <si>
+    <t>Asignación de cargos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-240A]\ #,##0"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,19 +774,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Garamond"/>
@@ -311,27 +790,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Georgia Pro Black"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Georgia Pro"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="3" tint="9.9978637043366805E-2"/>
-      <name val="Georgia Pro"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="6" tint="-0.249977111117893"/>
-      <name val="Georgia Pro"/>
       <family val="1"/>
     </font>
     <font>
@@ -360,8 +818,69 @@
       <name val="Georgia Pro Black"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="9.9978637043366805E-2"/>
+      <name val="Georgia Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Georgia Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Georgia Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Georgia Pro"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +890,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,7 +912,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -396,21 +921,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -458,47 +968,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,103 +1527,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D9117-F19F-4DD0-B7E0-678E6E9A8AE8}">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="6" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="12.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="2.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="30.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="3" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="13"/>
+    <row r="1" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="M2" s="23"/>
+    </row>
+    <row r="3" spans="2:14" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="37" t="s">
         <v>9</v>
       </c>
+      <c r="L7" s="38"/>
+      <c r="M7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="35" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="2:10" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="10" t="s">
-        <v>10</v>
-      </c>
+    <row r="8" spans="2:14" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="36"/>
     </row>
-    <row r="4" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
-        <v>6</v>
+    <row r="9" spans="2:14" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:10" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>4</v>
-      </c>
+    <row r="10" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="16"/>
     </row>
-    <row r="8" spans="2:10" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E7:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A9DF69-BE07-44B6-90FA-BDAF1006A025}">
+  <dimension ref="B1:M11"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
+    <col min="4" max="5" width="27.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="30.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="3" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="44"/>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="M2" s="23"/>
+    </row>
+    <row r="3" spans="2:13" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="45"/>
+      <c r="C3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Gestión de organigrama y de cargos creada
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/appointments/Appointments.xlsx
+++ b/src/main/resources/reports/appointments/Appointments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS DOCUMENTOS\CIADTI\PROYECTOS\SERVICIOS\CARGA TRABAJO\ciadti-especifico-carga-trabajo-services\src\main\resources\reports\appointments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F08F6C3-CB0C-4339-86A9-B4D099C5C994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B43814-9457-4E6F-90E8-79F3DD1E6B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle por dependencia" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="N9");
+jx:area(lastCell="O9");
 jx:image(src="logo" lastCell="B3" imageType="PNG");</t>
         </r>
       </text>
@@ -87,7 +87,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:mergeCells(cols="totalCompensations+11" rows="1" minCols="1" minRows="1" lastCell="C2");</t>
+jx:mergeCells(cols="totalCompensations+12" rows="1" minCols="1" minRows="1" lastCell="C2");</t>
         </r>
       </text>
     </comment>
@@ -111,7 +111,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:mergeCells(cols="totalCompensations+11" rows="1" minCols="1" minRows="1" lastCell="C3");</t>
+jx:mergeCells(cols="totalCompensations+12" rows="1" minCols="1" minRows="1" lastCell="C3");</t>
         </r>
       </text>
     </comment>
@@ -135,56 +135,56 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:mergeCells(cols="totalCompensations + 12" rows="1" minCols="1" minRows="1" lastCell="B5");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{8722B099-0860-40A0-B269-49C91B659DA8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="categories" var="category" lastCell="M8" direction="RIGHT");
-jx:merge(cols="size(category.compensaciones)" rows="1" minCols="1" minRows="1" lastCell="M7");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{ADEBB074-C394-40AA-9F56-576C504E5E64}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="category.compensaciones" var="compensation" lastCell="M8" direction="RIGHT");</t>
+jx:mergeCells(cols="totalCompensations + 13" rows="1" minCols="1" minRows="1" lastCell="B5");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{8722B099-0860-40A0-B269-49C91B659DA8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="categories" var="category" lastCell="N8" direction="RIGHT");
+jx:merge(cols="size(category.compensaciones)" rows="1" minCols="1" minRows="1" lastCell="N7");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{ADEBB074-C394-40AA-9F56-576C504E5E64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="category.compensaciones" var="compensation" lastCell="N8" direction="RIGHT");</t>
         </r>
       </text>
     </comment>
@@ -208,176 +208,200 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:eachMerge(items="dataset" var="scope" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{F5319C88-801F-4C8B-91D8-BE1A2647869F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:eachMerge(items="scope.children" var="validity" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{92997C66-2D07-4B7C-82E2-6BF7A0CE4182}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:eachMerge(items="validity.children" var="structure" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{0A3A7BAB-F781-4C63-9B7F-CBA921529458}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:eachMerge(items="structure.children" var="structureAppointment" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{BBA8CB56-BCD3-429D-B8F2-AFB6026544C4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:eachMerge(items="structureAppointment.children" var="normativity" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{CF9ED112-5F62-4EBF-921E-19DDB76428CE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:eachMerge(items="normativity.children" var="level" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{6414266E-9A2C-4C4C-9C05-2982714FE18C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:eachMerge(items="level.children" var="salaryScale" lastCell="N9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{305A5962-8E28-44AF-9F10-2329723ED3BA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="categories" var="category" lastCell="M9" direction="RIGHT");
-jx:each(items="category.compensaciones" var="compensation" lastCell="M9" direction="RIGHT");</t>
+jx:eachMerge(items="dataset" var="organizationChart" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{A96B944C-9F63-4236-8D77-820E3E99E05D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="organizationChart.children" var="scope" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{F5319C88-801F-4C8B-91D8-BE1A2647869F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="scope.children" var="validity" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{92997C66-2D07-4B7C-82E2-6BF7A0CE4182}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="validity.children" var="dependency" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{0A3A7BAB-F781-4C63-9B7F-CBA921529458}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="dependency.children" var="dependencyAppointment" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{BBA8CB56-BCD3-429D-B8F2-AFB6026544C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="dependencyAppointment.children" var="normativity" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{CF9ED112-5F62-4EBF-921E-19DDB76428CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="normativity.children" var="level" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{6414266E-9A2C-4C4C-9C05-2982714FE18C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:eachMerge(items="level.children" var="salaryScale" lastCell="O9")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{305A5962-8E28-44AF-9F10-2329723ED3BA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="categories" var="category" lastCell="N9" direction="RIGHT");
+jx:each(items="category.compensaciones" var="compensation" lastCell="N9" direction="RIGHT");</t>
         </r>
       </text>
     </comment>
@@ -411,7 +435,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="E11");
+jx:area(lastCell="E12");
 jx:image(src="logo" lastCell="B3" imageType="PNG");</t>
         </r>
       </text>
@@ -488,124 +512,149 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{CE9FAC1D-BF4D-4985-A473-EB1ECCA82FE5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="comparativesByScope" var="comparativeAttribute" lastCell="E8" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{1DD28C3D-ACC9-4964-9217-B9872A9CDD8E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="comparativeDataset" var="structure" lastCell="E11");
-jx:merge(cols="1 + size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="B9");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{1E3CEE09-E857-4793-B7B4-386B1C57C35C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="structure.children" var="level" lastCell="E10")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{CBA3538E-43DD-44C1-A687-0484FB8FE2BC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="level.comparativesByScope" var="comparativeAttribute" lastCell="E10" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{558F7C05-BE3B-49DC-8394-F1B8703199AA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronald Torres:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="comparativesByScope" var="comparativeAttribute" lastCell="E11" direction="RIGHT");</t>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{D2834268-5E23-4F5B-A8FC-3472AE795492}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="comparativeDataset" var="organizationChart" lastCell="E12");
+jx:merge(cols="1 + size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="B7");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{CE9FAC1D-BF4D-4985-A473-EB1ECCA82FE5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="comparativesByScope" var="comparativeAttribute" lastCell="E9" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{1DD28C3D-ACC9-4964-9217-B9872A9CDD8E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="organizationChart.children" var="dependency" lastCell="E12");
+jx:merge(cols="1 + size(comparativesByScope)*3" rows="1" minCols="1" minRows="1" lastCell="B10");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{1E3CEE09-E857-4793-B7B4-386B1C57C35C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="dependency.children" var="level" lastCell="E11")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{CBA3538E-43DD-44C1-A687-0484FB8FE2BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="level.comparativesByScope" var="comparativeAttribute" lastCell="E11" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{558F7C05-BE3B-49DC-8394-F1B8703199AA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronald Torres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="comparativesByScope" var="comparativeAttribute" lastCell="E12" direction="RIGHT");</t>
         </r>
       </text>
     </comment>
@@ -614,7 +663,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Fecha del reporte:  ${reportDate}</t>
   </si>
@@ -652,9 +701,6 @@
     <t>${validity.data.nombre}</t>
   </si>
   <si>
-    <t>${structure.data.nombre}</t>
-  </si>
-  <si>
     <t>${normativity.data.nombre}</t>
   </si>
   <si>
@@ -670,18 +716,9 @@
     <t>TOTAL DE CARGOS</t>
   </si>
   <si>
-    <t>$[K9*12]</t>
-  </si>
-  <si>
-    <t>$[UPPER(${"\"" +scope.data.nombre + "\""})]</t>
-  </si>
-  <si>
     <t>${compensation.nombre}</t>
   </si>
   <si>
-    <t>${structureAppointment.totalCargos}</t>
-  </si>
-  <si>
     <t>${salaryScale.totalCargos}</t>
   </si>
   <si>
@@ -703,12 +740,6 @@
     <t>TOTAL ANUAL</t>
   </si>
   <si>
-    <t>$[SUM(M9, L9)*J9]</t>
-  </si>
-  <si>
-    <t>$[UPPER(${"\"" +structure.data.nombre + "\""})]</t>
-  </si>
-  <si>
     <t>${level.data.nombre}</t>
   </si>
   <si>
@@ -724,25 +755,49 @@
     <t>${comparativeAttribute.asignacionBasicaAnual}</t>
   </si>
   <si>
-    <t>$[D10/12]</t>
-  </si>
-  <si>
     <t>Comparativo de costos por alcances operativos en las dependencias por niveles ocupacionales</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>${R.sumComparativesByScope(structure.children, comparativeAttribute.key, 'asignacionBasicaAnual')}</t>
-  </si>
-  <si>
-    <t>${R.sumComparativesByScope(structure.children, comparativeAttribute.key, 'totalCargos')}</t>
-  </si>
-  <si>
     <t>$[D11/12]</t>
   </si>
   <si>
     <t>Asignación de cargos</t>
+  </si>
+  <si>
+    <t>ESTRUCTURA ORGANIZACIONAL</t>
+  </si>
+  <si>
+    <t>$[UPPER(${"\"" +organizationChart.data.nombre + "\""})]</t>
+  </si>
+  <si>
+    <t>${scope.data.nombre}</t>
+  </si>
+  <si>
+    <t>${dependency.data.nombre}</t>
+  </si>
+  <si>
+    <t>${dependencyAppointment.totalCargos}</t>
+  </si>
+  <si>
+    <t>$[L9*12]</t>
+  </si>
+  <si>
+    <t>$[SUM(N9, M9)*K9]</t>
+  </si>
+  <si>
+    <t>$[UPPER(${"\"" +dependency.data.nombre + "\""})]</t>
+  </si>
+  <si>
+    <t>$[D12/12]</t>
+  </si>
+  <si>
+    <t>${R.sumComparativesByScope(dependency.children, comparativeAttribute.key, 'totalCargos')}</t>
+  </si>
+  <si>
+    <t>${R.sumComparativesByScope(dependency.children, comparativeAttribute.key, 'asignacionBasicaAnual')}</t>
   </si>
 </sst>
 </file>
@@ -1142,6 +1197,9 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1180,9 +1238,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,173 +1582,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D9117-F19F-4DD0-B7E0-678E6E9A8AE8}">
-  <dimension ref="B1:N13"/>
+  <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="30.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="3" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" style="16" customWidth="1"/>
-    <col min="14" max="14" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="3" width="45.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="3" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="3" customWidth="1"/>
+    <col min="12" max="13" width="20.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" style="16" customWidth="1"/>
+    <col min="15" max="15" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="M2" s="23"/>
+        <v>33</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="N2" s="23"/>
     </row>
-    <row r="3" spans="2:14" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
       <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="M3" s="24"/>
+      <c r="E3" s="11"/>
+      <c r="N3" s="24"/>
     </row>
-    <row r="4" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+    <row r="6" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:15" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="D7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="E7" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="F7" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="39"/>
+      <c r="N7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="38"/>
-      <c r="M7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="35" t="s">
-        <v>28</v>
-      </c>
+      <c r="O8" s="37"/>
     </row>
-    <row r="8" spans="2:14" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="14" t="s">
+    <row r="9" spans="2:15" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="36"/>
+      <c r="O9" s="25" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="2:14" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M13" s="16"/>
+    <row r="10" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1702,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A9DF69-BE07-44B6-90FA-BDAF1006A025}">
-  <dimension ref="B1:M11"/>
+  <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1726,17 +1789,17 @@
   <sheetData>
     <row r="1" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="44"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D2" s="10"/>
       <c r="M2" s="23"/>
     </row>
     <row r="3" spans="2:13" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D3" s="11"/>
       <c r="M3" s="24"/>
@@ -1748,65 +1811,70 @@
       </c>
     </row>
     <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
+    <row r="7" spans="2:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="32" t="s">
+      <c r="B8" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="C9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="9" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="26" t="s">
+    <row r="12" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>41</v>
+      <c r="C12" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Asignación de cargos por denominación de empleo y orden de los niveles en los reportes
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/appointments/Appointments.xlsx
+++ b/src/main/resources/reports/appointments/Appointments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS DOCUMENTOS\CIADTI\PROYECTOS\SERVICIOS\CARGA TRABAJO\ciadti-especifico-carga-trabajo-services\src\main\resources\reports\appointments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B43814-9457-4E6F-90E8-79F3DD1E6B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A014F1FE-5407-4FE6-AD7D-BEB07519D9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle por dependencia" sheetId="2" r:id="rId1"/>
@@ -689,9 +689,6 @@
     <t>ESCALA SALARIAL</t>
   </si>
   <si>
-    <t>CÓDIGO</t>
-  </si>
-  <si>
     <t>ASIGNACIÓN</t>
   </si>
   <si>
@@ -710,9 +707,6 @@
     <t>${salaryScale.data.nombre}</t>
   </si>
   <si>
-    <t>${salaryScale.data.codigo}</t>
-  </si>
-  <si>
     <t>TOTAL DE CARGOS</t>
   </si>
   <si>
@@ -798,6 +792,12 @@
   </si>
   <si>
     <t>${R.sumComparativesByScope(dependency.children, comparativeAttribute.key, 'asignacionBasicaAnual')}</t>
+  </si>
+  <si>
+    <t>DENOMINACIONES DE EMPLEOS</t>
+  </si>
+  <si>
+    <t>${salaryScale.detallesDenominacionesEmpleos}</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1160,9 +1160,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1585,7 +1582,7 @@
   <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+      <selection activeCell="BG5" sqref="BG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1594,7 @@
     <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="40.7109375" style="3" customWidth="1"/>
     <col min="8" max="9" width="30.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="44.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" style="3" customWidth="1"/>
     <col min="12" max="13" width="20.7109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="40.7109375" style="16" customWidth="1"/>
@@ -1609,10 +1606,10 @@
     <row r="2" spans="2:15" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="N2" s="23"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="2:15" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
@@ -1620,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="11"/>
-      <c r="N3" s="24"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1630,111 +1627,111 @@
     </row>
     <row r="6" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:15" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="34" t="s">
+      <c r="D7" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="34" t="s">
+      <c r="F7" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="39"/>
+      <c r="M7" s="38"/>
       <c r="N7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="36" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="O7" s="35" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:15" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="41"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="40"/>
       <c r="L8" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="37"/>
+        <v>15</v>
+      </c>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="2:15" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="F9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="G9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="H9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="N9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="O9" s="25" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1789,20 +1786,20 @@
   <sheetData>
     <row r="1" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="45"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="M2" s="23"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="2:13" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="46"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="M3" s="24"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1813,62 +1810,62 @@
     <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
+      <c r="C8" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>21</v>
+      <c r="B9" s="34"/>
+      <c r="C9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
-        <v>41</v>
+      <c r="B10" s="32" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>32</v>
+      <c r="B11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="31" t="s">
+      <c r="B12" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="30" t="s">
         <v>42</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>